<commit_message>
make equations optional for MCP and CNS models
</commit_message>
<xml_diff>
--- a/tests/integration/models/results.xlsx
+++ b/tests/integration/models/results.xlsx
@@ -3691,19 +3691,19 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>253.9999550208449</v>
+        <v>258.0000087618828</v>
       </c>
       <c r="E26" t="n">
-        <v>239.0005392953753</v>
+        <v>237.9997400566936</v>
       </c>
       <c r="F26" t="n">
-        <v>234.9998569115996</v>
+        <v>237.0001981034875</v>
       </c>
       <c r="G26" t="n">
-        <v>209.9999925121665</v>
+        <v>210.9995344653726</v>
       </c>
       <c r="H26" t="n">
-        <v>211.0001631081104</v>
+        <v>208.0002799630165</v>
       </c>
     </row>
     <row r="27">

</xml_diff>